<commit_message>
Inicialización de la base de datos
</commit_message>
<xml_diff>
--- a/Reporte_Empleados.xlsx
+++ b/Reporte_Empleados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,6 +731,62 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Jos</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Armas</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Coyo</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1234455</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>jospspd</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>kaddkdakakd</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1987-12-01</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>